<commit_message>
Add definitive layer rules to prevent confusion
</commit_message>
<xml_diff>
--- a/templates/walkthroughs/Bronze_Walkthrough.xlsx
+++ b/templates/walkthroughs/Bronze_Walkthrough.xlsx
@@ -23,7 +23,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="16">
+  <fonts count="18">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -86,16 +86,24 @@
     </font>
     <font>
       <b val="1"/>
+      <color rgb="001F4E79"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <i val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00006100"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
       <color rgb="00C00000"/>
       <sz val="12"/>
     </font>
     <font>
       <color rgb="00C00000"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00006100"/>
-      <sz val="12"/>
     </font>
   </fonts>
   <fills count="7">
@@ -154,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -179,6 +187,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -5374,7 +5384,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5388,91 +5398,133 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>REFERENCE - BRONZE PATTERNS</t>
+          <t>REFERENCE - BRONZE LAYER RULES</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="16" t="inlineStr">
         <is>
-          <t>ANTI-PATTERNS</t>
+          <t>BRONZE = YOUR UNDO BUTTON</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="17" t="inlineStr">
         <is>
-          <t>❌ Transforming or cleaning data</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="17" t="inlineStr">
-        <is>
-          <t>❌ Filtering business rows</t>
+          <t>If something goes wrong downstream, you can always reprocess from Bronze.</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="17" t="inlineStr">
-        <is>
-          <t>❌ Joining tables</t>
+      <c r="A6" s="18" t="inlineStr">
+        <is>
+          <t>✅ ALLOWED IN BRONZE</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="17" t="inlineStr">
-        <is>
-          <t>❌ Using Merge pattern</t>
+      <c r="A7" s="19" t="inlineStr">
+        <is>
+          <t>✅ Land data exactly as-is from source</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="17" t="inlineStr">
-        <is>
-          <t>❌ Not adding _extracted_at</t>
+      <c r="A8" s="19" t="inlineStr">
+        <is>
+          <t>✅ Append mode only (accumulate history)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="19" t="inlineStr">
+        <is>
+          <t>✅ Add metadata columns (_extracted_at, _batch_id, _source_file)</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="18" t="inlineStr">
-        <is>
-          <t>BEST PRACTICES</t>
+      <c r="A10" s="19" t="inlineStr">
+        <is>
+          <t>✅ Schema evolution (allow new columns)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="19" t="inlineStr">
         <is>
-          <t>✅ Land data as-is</t>
+          <t>✅ Smart Read (rolling_window, stateful) for incremental</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="19" t="inlineStr">
         <is>
-          <t>✅ Always APPEND mode</t>
+          <t>✅ Route bad records to quarantine path</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="19" t="inlineStr">
         <is>
-          <t>✅ Add _extracted_at metadata</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="19" t="inlineStr">
-        <is>
-          <t>✅ Use Smart Read for incremental</t>
+          <t>✅ Duplicates are expected - Silver handles them</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="19" t="inlineStr">
-        <is>
-          <t>✅ Let Silver deduplicate</t>
+      <c r="A15" s="20" t="inlineStr">
+        <is>
+          <t>❌ NOT ALLOWED IN BRONZE</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="21" t="inlineStr">
+        <is>
+          <t>❌ Any data transformation</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="21" t="inlineStr">
+        <is>
+          <t>❌ Merge, upsert, or overwrite modes</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="21" t="inlineStr">
+        <is>
+          <t>❌ Filter or remove rows</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="21" t="inlineStr">
+        <is>
+          <t>❌ Clean or standardize data</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="21" t="inlineStr">
+        <is>
+          <t>❌ Join any tables</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="21" t="inlineStr">
+        <is>
+          <t>❌ Apply business logic</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="21" t="inlineStr">
+        <is>
+          <t>❌ Deduplicate</t>
         </is>
       </c>
     </row>

</xml_diff>